<commit_message>
ignore this accidental change to excel file
</commit_message>
<xml_diff>
--- a/comoOdeCpp/tests/testthat/data/templates_v19.1/Template_CoMoCOVID-19App_v19_all_interventions.xlsx
+++ b/comoOdeCpp/tests/testthat/data/templates_v19.1/Template_CoMoCOVID-19App_v19_all_interventions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowHeight="17850" tabRatio="648" firstSheet="2" activeTab="10"/>
+    <workbookView windowHeight="17850" tabRatio="648" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -3213,12 +3213,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="0.0"/>
+    <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="0.0"/>
   </numFmts>
   <fonts count="40">
     <font>
@@ -3336,6 +3336,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -3344,8 +3358,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3360,9 +3383,25 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3374,17 +3413,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3399,7 +3443,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3412,60 +3456,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3476,6 +3468,14 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3572,7 +3572,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3584,13 +3620,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3602,85 +3662,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3698,7 +3680,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3710,37 +3722,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3858,6 +3858,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -3879,21 +3894,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -3904,6 +3904,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3922,155 +3931,146 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="19" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="31" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="19" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="16" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4248,7 +4248,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4284,10 +4284,10 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -4300,7 +4300,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -5781,8 +5781,8 @@
   </sheetPr>
   <dimension ref="A1:G78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8733333333333" defaultRowHeight="15.75" outlineLevelCol="6"/>
@@ -6954,11 +6954,11 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A18 G5:G18">
+      <formula1>[1]HIDDEN!#REF!</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2 G3 G4 G19:G78">
       <formula1>HIDDEN!$I$2:$I$3</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A18 G5:G18">
-      <formula1>[1]HIDDEN!#REF!</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2 D3 D4 D5:D18 D19:D78">
       <formula1>0</formula1>
@@ -9676,8 +9676,8 @@
   </sheetPr>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8733333333333" defaultRowHeight="15.75" outlineLevelCol="5"/>

</xml_diff>